<commit_message>
aggiornati file xls e data
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/accreditamento-checklist_V8.2.5.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/accreditamento-checklist_V8.2.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CFB7F5-333C-4451-967D-EFB0B2F0C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0F1690-E625-4A00-B627-882C1A29F93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="705" windowWidth="24630" windowHeight="14385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="707">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3298,6 +3298,9 @@
   </si>
   <si>
     <t>2025-05-14T15:12:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -5367,7 +5370,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S169" sqref="S169:S170"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5447,6 +5450,9 @@
         <v>436</v>
       </c>
       <c r="D3" s="47"/>
+      <c r="E3" t="s">
+        <v>706</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -5472,6 +5478,9 @@
         <v>437</v>
       </c>
       <c r="D4" s="47"/>
+      <c r="E4" t="s">
+        <v>706</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -5497,6 +5506,9 @@
         <v>438</v>
       </c>
       <c r="D5" s="47"/>
+      <c r="E5" t="s">
+        <v>706</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -20548,27 +20560,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20826,32 +20817,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20868,4 +20855,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>